<commit_message>
Updated UIS strategy to US Markets rather than QQQ
</commit_message>
<xml_diff>
--- a/Optimzations-burdin2.xlsx
+++ b/Optimzations-burdin2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\LogicalInvest\git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA168397-791D-4CC5-90D1-7C93CEAF881A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1179CC27-B919-40D7-ACE6-86122B6C14B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="16920" windowHeight="9560" xr2:uid="{109E868A-4B1B-4E85-97C8-089867AD6957}"/>
+    <workbookView xWindow="16935" yWindow="1080" windowWidth="20025" windowHeight="12555" xr2:uid="{109E868A-4B1B-4E85-97C8-089867AD6957}"/>
   </bookViews>
   <sheets>
     <sheet name="Joint" sheetId="1" r:id="rId1"/>
@@ -176,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -243,6 +243,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,276 +558,273 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8690D2E-C911-40D4-BA06-A8C107F8685B}">
-  <dimension ref="A1:G103"/>
+  <dimension ref="A1:G104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="63.7265625" style="1" customWidth="1"/>
-    <col min="2" max="4" width="9.1796875" style="1"/>
-    <col min="5" max="5" width="12.81640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.453125" style="21" customWidth="1"/>
-    <col min="7" max="7" width="15.36328125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="63.7109375" style="1" customWidth="1"/>
+    <col min="2" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="12.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" style="21" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="26">
+        <v>44928</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F2" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+    <row r="3" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B3" s="5">
         <v>20.399000000000001</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C3" s="5">
         <v>1.89</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D3" s="5">
         <v>17.154</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E3" s="5">
         <v>-35.020000000000003</v>
       </c>
-      <c r="F2" s="13"/>
-    </row>
-    <row r="3" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="22" t="s">
+      <c r="F3" s="13"/>
+    </row>
+    <row r="4" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="5">
-        <v>15.284000000000001</v>
-      </c>
-      <c r="C3" s="5">
-        <v>1.5820000000000001</v>
-      </c>
-      <c r="D3" s="5">
-        <v>9.66</v>
-      </c>
-      <c r="E3" s="5">
-        <v>-8.61</v>
-      </c>
-      <c r="F3" s="13">
+      <c r="B4" s="5">
+        <v>14.24</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1.377</v>
+      </c>
+      <c r="D4" s="5">
+        <v>10.343999999999999</v>
+      </c>
+      <c r="E4" s="5">
+        <v>-10.23</v>
+      </c>
+      <c r="F4" s="13">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="23" t="s">
+    <row r="5" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>11.871</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>1.3029999999999999</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <v>9.11</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <v>-10.39</v>
       </c>
-      <c r="F4" s="24">
+      <c r="F5" s="24">
         <v>0.5</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="7" t="s">
+    <row r="6" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B6" s="5">
         <v>20.696999999999999</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C6" s="5">
         <v>1.272</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D6" s="5">
         <v>16.265000000000001</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E6" s="5">
         <v>-23.46</v>
       </c>
-      <c r="F5" s="13"/>
-    </row>
-    <row r="6" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="7" t="s">
+      <c r="F6" s="13"/>
+    </row>
+    <row r="7" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B7" s="5">
         <v>22.058</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C7" s="5">
         <v>1.202</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D7" s="5">
         <v>18.344999999999999</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E7" s="5">
         <v>-35.020000000000003</v>
       </c>
-      <c r="F6" s="13"/>
-    </row>
-    <row r="7" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
+      <c r="F7" s="13"/>
+    </row>
+    <row r="8" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B8" s="5">
         <v>23.571000000000002</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C8" s="5">
         <v>1.181</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D8" s="5">
         <v>19.960999999999999</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E8" s="5">
         <v>-26.13</v>
       </c>
-      <c r="F7" s="13"/>
-    </row>
-    <row r="8" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="7" t="s">
+      <c r="F8" s="13"/>
+    </row>
+    <row r="9" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B9" s="5">
         <v>10.738</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C9" s="5">
         <v>1.1339999999999999</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D9" s="5">
         <v>9.468</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E9" s="5">
         <v>-14.16</v>
       </c>
-      <c r="F8" s="13"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="7" t="s">
+      <c r="F9" s="13"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B10" s="5">
         <v>4.1470000000000002</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C10" s="5">
         <v>1.1100000000000001</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D10" s="5">
         <v>3.7360000000000002</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E10" s="5">
         <v>-8.02</v>
       </c>
-      <c r="F9" s="25">
+      <c r="F10" s="25">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B11" s="5">
         <v>8.8000000000000007</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C11" s="5">
         <v>0.90600000000000003</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D11" s="5">
         <v>9.7210000000000001</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E11" s="5">
         <v>-24.61</v>
       </c>
-      <c r="F10" s="14"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="7" t="s">
+      <c r="F11" s="14"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B12" s="5">
         <v>13.397</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C12" s="5">
         <v>0.623</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D12" s="5">
         <v>21.509</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E12" s="5">
         <v>-53.4</v>
       </c>
-      <c r="F11" s="13"/>
-    </row>
-    <row r="12" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="9" t="s">
+      <c r="F12" s="13"/>
+    </row>
+    <row r="13" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B13" s="5">
         <v>9.2759999999999998</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C13" s="5">
         <v>0.48</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D13" s="5">
         <v>19.312999999999999</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E13" s="5">
         <v>-55.19</v>
       </c>
-      <c r="F12" s="15"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="7" t="s">
+      <c r="F13" s="15"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B14" s="5">
         <v>9.4149999999999991</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C14" s="5">
         <v>0.40100000000000002</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D14" s="5">
         <v>23.475000000000001</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E14" s="5">
         <v>-58.69</v>
       </c>
-      <c r="F13" s="13"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="2"/>
-      <c r="B14"/>
-      <c r="C14"/>
-      <c r="D14"/>
-      <c r="E14"/>
-      <c r="F14" s="16"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F14" s="13"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15"/>
       <c r="C15"/>
@@ -834,7 +832,7 @@
       <c r="E15"/>
       <c r="F15" s="16"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16"/>
       <c r="C16"/>
@@ -842,7 +840,7 @@
       <c r="E16"/>
       <c r="F16" s="16"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17"/>
       <c r="C17"/>
@@ -850,7 +848,7 @@
       <c r="E17"/>
       <c r="F17" s="16"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18"/>
       <c r="C18"/>
@@ -858,7 +856,7 @@
       <c r="E18"/>
       <c r="F18" s="16"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19"/>
       <c r="C19"/>
@@ -866,15 +864,15 @@
       <c r="E19"/>
       <c r="F19" s="16"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20"/>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
       <c r="B20"/>
       <c r="C20"/>
       <c r="D20"/>
       <c r="E20"/>
-      <c r="F20" s="17"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F20" s="16"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
@@ -882,15 +880,15 @@
       <c r="E21"/>
       <c r="F21" s="17"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="2"/>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
       <c r="D22"/>
       <c r="E22"/>
-      <c r="F22" s="16"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F22" s="17"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23"/>
       <c r="C23"/>
@@ -898,7 +896,7 @@
       <c r="E23"/>
       <c r="F23" s="16"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24"/>
       <c r="C24"/>
@@ -906,15 +904,15 @@
       <c r="E24"/>
       <c r="F24" s="16"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25"/>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
       <c r="B25"/>
       <c r="C25"/>
       <c r="D25"/>
       <c r="E25"/>
-      <c r="F25" s="17"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F25" s="16"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26"/>
       <c r="B26"/>
       <c r="C26"/>
@@ -922,15 +920,15 @@
       <c r="E26"/>
       <c r="F26" s="17"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="2"/>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27"/>
       <c r="B27"/>
       <c r="C27"/>
       <c r="D27"/>
       <c r="E27"/>
-      <c r="F27" s="16"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F27" s="17"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28"/>
       <c r="C28"/>
@@ -938,7 +936,7 @@
       <c r="E28"/>
       <c r="F28" s="16"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29"/>
       <c r="C29"/>
@@ -946,7 +944,7 @@
       <c r="E29"/>
       <c r="F29" s="16"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30"/>
       <c r="C30"/>
@@ -954,241 +952,249 @@
       <c r="E30"/>
       <c r="F30" s="16"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="8"/>
-      <c r="F31" s="18"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="8"/>
-      <c r="F33" s="18"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31"/>
+      <c r="C31"/>
+      <c r="D31"/>
+      <c r="E31"/>
+      <c r="F31" s="16"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="8"/>
+      <c r="F32" s="18"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="F34" s="18"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="F35" s="18"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="F36" s="18"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="F37" s="18"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="F38" s="18"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="F39" s="18"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="F40" s="18"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A43" s="8"/>
-      <c r="F43" s="18"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="8"/>
+      <c r="F41" s="18"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="F44" s="18"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
       <c r="F45" s="18"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="F46" s="18"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="8"/>
       <c r="F47" s="18"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A50" s="8"/>
-      <c r="F50" s="18"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="8"/>
+      <c r="F48" s="18"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="8"/>
       <c r="F51" s="18"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="8"/>
       <c r="F52" s="18"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A54" s="8"/>
-      <c r="F54" s="18"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="8"/>
+      <c r="F53" s="18"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="8"/>
       <c r="F55" s="18"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="8"/>
       <c r="F56" s="18"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="8"/>
       <c r="F57" s="18"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="8"/>
       <c r="F58" s="18"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="8"/>
       <c r="F59" s="18"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="8"/>
       <c r="F60" s="18"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="8"/>
       <c r="F61" s="18"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A63" s="8"/>
-      <c r="F63" s="18"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="8"/>
+      <c r="F62" s="18"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="8"/>
       <c r="F64" s="18"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="8"/>
       <c r="F65" s="18"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A67" s="8"/>
-      <c r="F67" s="18"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="8"/>
+      <c r="F66" s="18"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="8"/>
       <c r="F68" s="18"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A69" s="11"/>
-      <c r="F69" s="19"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A71" s="8"/>
-      <c r="F71" s="18"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="8"/>
+      <c r="F69" s="18"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="11"/>
+      <c r="F70" s="19"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="8"/>
       <c r="F72" s="18"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="8"/>
       <c r="F73" s="18"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A74" s="7"/>
-      <c r="F74" s="13"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A75" s="10"/>
-      <c r="F75" s="20"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A76" s="8"/>
-      <c r="F76" s="18"/>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="8"/>
+      <c r="F74" s="18"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="7"/>
+      <c r="F75" s="13"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="10"/>
+      <c r="F76" s="20"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="8"/>
       <c r="F77" s="18"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="8"/>
       <c r="F78" s="18"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A81" s="8"/>
-      <c r="F81" s="18"/>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="8"/>
+      <c r="F79" s="18"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="8"/>
       <c r="F82" s="18"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="8"/>
       <c r="F83" s="18"/>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="8"/>
       <c r="F84" s="18"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="8"/>
       <c r="F85" s="18"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A86" s="7"/>
-      <c r="F86" s="13"/>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A87" s="8"/>
-      <c r="F87" s="18"/>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="8"/>
+      <c r="F86" s="18"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="7"/>
+      <c r="F87" s="13"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="8"/>
       <c r="F88" s="18"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="8"/>
       <c r="F89" s="18"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="8"/>
       <c r="F90" s="18"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A92" s="8"/>
-      <c r="F92" s="18"/>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="8"/>
+      <c r="F91" s="18"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="8"/>
       <c r="F93" s="18"/>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A95" s="9"/>
-      <c r="F95" s="15"/>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A96" s="8"/>
-      <c r="F96" s="18"/>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A98" s="9"/>
-      <c r="F98" s="15"/>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A99" s="8"/>
-      <c r="F99" s="18"/>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A101" s="9"/>
-      <c r="F101" s="15"/>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A102" s="8"/>
-      <c r="F102" s="18"/>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="8"/>
+      <c r="F94" s="18"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="9"/>
+      <c r="F96" s="15"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="8"/>
+      <c r="F97" s="18"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" s="9"/>
+      <c r="F99" s="15"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="8"/>
+      <c r="F100" s="18"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" s="9"/>
+      <c r="F102" s="15"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="8"/>
       <c r="F103" s="18"/>
     </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" s="8"/>
+      <c r="F104" s="18"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F103">
-    <sortCondition descending="1" ref="C1:C103"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:F104">
+    <sortCondition descending="1" ref="C2:C104"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>
@@ -1203,19 +1209,19 @@
       <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
@@ -1232,7 +1238,7 @@
         <v>-45.65</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>15</v>
       </c>
@@ -1249,7 +1255,7 @@
         <v>-24.26</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>16</v>
       </c>
@@ -1266,10 +1272,10 @@
         <v>-21.79</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>19</v>
       </c>
@@ -1286,7 +1292,7 @@
         <v>-13.95</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>0</v>
       </c>
@@ -1303,7 +1309,7 @@
         <v>-17.38</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>17</v>
       </c>
@@ -1320,10 +1326,10 @@
         <v>-25.21</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1340,7 +1346,7 @@
         <v>-31.87</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -1357,7 +1363,7 @@
         <v>-51.68</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>7</v>
       </c>

</xml_diff>